<commit_message>
v2.6 - add calculating format
</commit_message>
<xml_diff>
--- a/dist/format.xlsx
+++ b/dist/format.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008560E5-CE9D-4B89-8749-AF5A5873D604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5496AB34-AEBB-4E46-B53F-CB86105A7E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="formats" sheetId="1" r:id="rId1"/>
@@ -624,7 +624,7 @@
         <v>13</v>
       </c>
       <c r="F11">
-        <v>5930</v>
+        <v>5990</v>
       </c>
       <c r="G11">
         <v>8475</v>

</xml_diff>